<commit_message>
Tutorial on unifrac ordination with VVKAJ
</commit_message>
<xml_diff>
--- a/eg_data/VVKAJ/ind_metadata_prep.xlsx
+++ b/eg_data/VVKAJ/ind_metadata_prep.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadoh\OneDrive\Documents\GitHub\dietary_patterns\eg_data\VVKAJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D754FF-87FC-4400-A31C-DD7A41628370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BAC5A5-2126-406A-A111-433A9DE9D84F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-3495" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20880" yWindow="-2985" windowWidth="20145" windowHeight="12315" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="metadata.txt" sheetId="2" r:id="rId2"/>
-    <sheet name="to rm" sheetId="3" r:id="rId3"/>
-    <sheet name="metadata_1miss.txt" sheetId="4" r:id="rId4"/>
+    <sheet name="User x Day" sheetId="5" r:id="rId3"/>
+    <sheet name="to rm" sheetId="3" r:id="rId4"/>
+    <sheet name="metadata_1miss.txt" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="86">
   <si>
     <t>UserName</t>
   </si>
@@ -146,6 +147,156 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>StudyDayNo</t>
+  </si>
+  <si>
+    <t>vvkaj.00001</t>
+  </si>
+  <si>
+    <t>vvkaj.00002</t>
+  </si>
+  <si>
+    <t>vvkaj.00003</t>
+  </si>
+  <si>
+    <t>vvkaj.00004</t>
+  </si>
+  <si>
+    <t>vvkaj.00005</t>
+  </si>
+  <si>
+    <t>vvkaj.00006</t>
+  </si>
+  <si>
+    <t>vvkaj.00007</t>
+  </si>
+  <si>
+    <t>vvkaj.00008</t>
+  </si>
+  <si>
+    <t>vvkaj.00009</t>
+  </si>
+  <si>
+    <t>vvkaj.00010</t>
+  </si>
+  <si>
+    <t>vvkaj.00011</t>
+  </si>
+  <si>
+    <t>vvkaj.00012</t>
+  </si>
+  <si>
+    <t>vvkaj.00013</t>
+  </si>
+  <si>
+    <t>vvkaj.00014</t>
+  </si>
+  <si>
+    <t>vvkaj.00015</t>
+  </si>
+  <si>
+    <t>vvkaj.00016</t>
+  </si>
+  <si>
+    <t>vvkaj.00017</t>
+  </si>
+  <si>
+    <t>vvkaj.00018</t>
+  </si>
+  <si>
+    <t>vvkaj.00019</t>
+  </si>
+  <si>
+    <t>vvkaj.00020</t>
+  </si>
+  <si>
+    <t>vvkaj.00021</t>
+  </si>
+  <si>
+    <t>vvkaj.00022</t>
+  </si>
+  <si>
+    <t>vvkaj.00023</t>
+  </si>
+  <si>
+    <t>vvkaj.00024</t>
+  </si>
+  <si>
+    <t>vvkaj.00025</t>
+  </si>
+  <si>
+    <t>vvkaj.00026</t>
+  </si>
+  <si>
+    <t>vvkaj.00027</t>
+  </si>
+  <si>
+    <t>vvkaj.00028</t>
+  </si>
+  <si>
+    <t>vvkaj.00029</t>
+  </si>
+  <si>
+    <t>vvkaj.00030</t>
+  </si>
+  <si>
+    <t>vvkaj.00031</t>
+  </si>
+  <si>
+    <t>vvkaj.00032</t>
+  </si>
+  <si>
+    <t>vvkaj.00033</t>
+  </si>
+  <si>
+    <t>vvkaj.00034</t>
+  </si>
+  <si>
+    <t>vvkaj.00035</t>
+  </si>
+  <si>
+    <t>vvkaj.00036</t>
+  </si>
+  <si>
+    <t>vvkaj.00037</t>
+  </si>
+  <si>
+    <t>vvkaj.00038</t>
+  </si>
+  <si>
+    <t>vvkaj.00039</t>
+  </si>
+  <si>
+    <t>vvkaj.00040</t>
+  </si>
+  <si>
+    <t>vvkaj.00041</t>
+  </si>
+  <si>
+    <t>vvkaj.00042</t>
+  </si>
+  <si>
+    <t>vvkaj.00043</t>
+  </si>
+  <si>
+    <t>vvkaj.00044</t>
+  </si>
+  <si>
+    <t>vvkaj.00045</t>
+  </si>
+  <si>
+    <t>vvkaj.00046</t>
+  </si>
+  <si>
+    <t>vvkaj.00047</t>
+  </si>
+  <si>
+    <t>vvkaj.00048</t>
+  </si>
+  <si>
+    <t>SampleID</t>
   </si>
 </sst>
 </file>
@@ -184,7 +335,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -192,11 +343,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -207,6 +438,21 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:H38"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,29 +1350,30 @@
         <v>25.848919068585648</v>
       </c>
     </row>
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="12" t="s">
         <v>6</v>
       </c>
       <c r="J22" t="s">
@@ -1137,28 +1384,28 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23">
+      <c r="C23" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="14">
         <v>25</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="14">
         <v>85</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="14">
         <v>169</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="14">
         <v>29.760862714890941</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="15">
         <v>89</v>
       </c>
       <c r="I23">
@@ -1169,28 +1416,28 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24">
+      <c r="C24" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="14">
         <v>62</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="14">
         <v>90.723500000000016</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="14">
         <v>161</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="14">
         <v>35</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="15">
         <v>110</v>
       </c>
       <c r="I24">
@@ -1204,28 +1451,28 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25">
+      <c r="C25" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="14">
         <v>29</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="14">
         <v>82.378399999999999</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="14">
         <v>178</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="14">
         <v>26</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="15">
         <v>91</v>
       </c>
       <c r="I25">
@@ -1236,28 +1483,28 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26">
+      <c r="C26" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="14">
         <v>38</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="14">
         <v>55</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="14">
         <v>152</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="14">
         <v>23.80540166204986</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="15">
         <v>78</v>
       </c>
       <c r="I26">
@@ -1268,28 +1515,28 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27">
+      <c r="C27" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="14">
         <v>47</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="14">
         <v>53.9</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="14">
         <v>161.30000000000001</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="14">
         <v>20.716673924549021</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="15">
         <v>85.5</v>
       </c>
       <c r="I27">
@@ -1300,28 +1547,28 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28">
+      <c r="C28" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="14">
         <v>60</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="14">
         <v>73</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="14">
         <v>163</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="14">
         <v>27.475629493018182</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="15">
         <v>90</v>
       </c>
       <c r="I28">
@@ -1332,28 +1579,28 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29">
+      <c r="C29" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="14">
         <v>48</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="14">
         <v>69.899200000000008</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="14">
         <v>158</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="14">
         <v>28</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="15">
         <v>95.5</v>
       </c>
       <c r="I29">
@@ -1367,28 +1614,28 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C30" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30">
+      <c r="C30" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="14">
         <v>53</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="14">
         <v>68</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="14">
         <v>159</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="14">
         <v>26.897670187097027</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="15">
         <v>85</v>
       </c>
       <c r="I30">
@@ -1399,28 +1646,28 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31">
+      <c r="C31" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="14">
         <v>28</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="14">
         <v>90.2</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="14">
         <v>181.3</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="14">
         <v>27.44169476499474</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="15">
         <v>95.5</v>
       </c>
       <c r="I31">
@@ -1431,28 +1678,28 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32">
+      <c r="C32" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="14">
         <v>71</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="14">
         <v>60</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="14">
         <v>169</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="14">
         <v>21.007667798746546</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="15">
         <v>75</v>
       </c>
       <c r="I32">
@@ -1463,28 +1710,28 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C33" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33">
+      <c r="C33" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="14">
         <v>22</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="14">
         <v>69.634799999999998</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="14">
         <v>174</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="14">
         <v>23</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="15">
         <v>70</v>
       </c>
       <c r="I33">
@@ -1498,28 +1745,28 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C34" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34">
+      <c r="C34" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="14">
         <v>43</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="14">
         <v>81</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="14">
         <v>175</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="14">
         <v>26.448979591836736</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="15">
         <v>72</v>
       </c>
       <c r="I34">
@@ -1530,28 +1777,28 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35">
+      <c r="C35" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="14">
         <v>43</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="14">
         <v>80</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="14">
         <v>183</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="14">
         <v>23.888440980620498</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="15">
         <v>98</v>
       </c>
       <c r="I35">
@@ -1565,28 +1812,28 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C36" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36">
+      <c r="C36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="14">
         <v>32</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="14">
         <v>59.4</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="14">
         <v>177.8</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="14">
         <v>18.789833498034341</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="15">
         <v>81</v>
       </c>
       <c r="I36">
@@ -1597,28 +1844,28 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C37" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37">
+      <c r="C37" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="14">
         <v>31</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="14">
         <v>79</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="14">
         <v>186</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="14">
         <v>22.835009827725745</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="15">
         <v>80</v>
       </c>
       <c r="I37">
@@ -1628,29 +1875,29 @@
         <v>22.835009827725745</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C38" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38">
+      <c r="C38" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="17">
         <v>60</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="17">
         <v>74.900000000000006</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="17">
         <v>164.1</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="17">
         <v>27.814077190934174</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="18">
         <v>78</v>
       </c>
       <c r="I38">
@@ -1679,7 +1926,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="A17" sqref="A1:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2141,6 +2388,1601 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{594EDA6F-1CFC-42B1-90D7-9924266EEBF7}">
+  <dimension ref="A1:J49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="20">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>31</v>
+      </c>
+      <c r="G2">
+        <v>79</v>
+      </c>
+      <c r="H2">
+        <v>186</v>
+      </c>
+      <c r="I2">
+        <v>22.835009827725745</v>
+      </c>
+      <c r="J2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="20">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>31</v>
+      </c>
+      <c r="G3">
+        <v>79</v>
+      </c>
+      <c r="H3">
+        <v>186</v>
+      </c>
+      <c r="I3">
+        <v>22.835009827725745</v>
+      </c>
+      <c r="J3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="20">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>31</v>
+      </c>
+      <c r="G4">
+        <v>79</v>
+      </c>
+      <c r="H4">
+        <v>186</v>
+      </c>
+      <c r="I4">
+        <v>22.835009827725745</v>
+      </c>
+      <c r="J4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="20">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>60</v>
+      </c>
+      <c r="G5">
+        <v>73</v>
+      </c>
+      <c r="H5">
+        <v>163</v>
+      </c>
+      <c r="I5">
+        <v>27.475629493018182</v>
+      </c>
+      <c r="J5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="20">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>60</v>
+      </c>
+      <c r="G6">
+        <v>73</v>
+      </c>
+      <c r="H6">
+        <v>163</v>
+      </c>
+      <c r="I6">
+        <v>27.475629493018182</v>
+      </c>
+      <c r="J6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="20">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>60</v>
+      </c>
+      <c r="G7">
+        <v>73</v>
+      </c>
+      <c r="H7">
+        <v>163</v>
+      </c>
+      <c r="I7">
+        <v>27.475629493018182</v>
+      </c>
+      <c r="J7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="20">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>43</v>
+      </c>
+      <c r="G8">
+        <v>81</v>
+      </c>
+      <c r="H8">
+        <v>175</v>
+      </c>
+      <c r="I8">
+        <v>26.448979591836736</v>
+      </c>
+      <c r="J8">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="20">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>43</v>
+      </c>
+      <c r="G9">
+        <v>81</v>
+      </c>
+      <c r="H9">
+        <v>175</v>
+      </c>
+      <c r="I9">
+        <v>26.448979591836736</v>
+      </c>
+      <c r="J9">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="20">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>43</v>
+      </c>
+      <c r="G10">
+        <v>81</v>
+      </c>
+      <c r="H10">
+        <v>175</v>
+      </c>
+      <c r="I10">
+        <v>26.448979591836736</v>
+      </c>
+      <c r="J10">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="19">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="5">
+        <v>25</v>
+      </c>
+      <c r="G11" s="5">
+        <v>85</v>
+      </c>
+      <c r="H11" s="5">
+        <v>169</v>
+      </c>
+      <c r="I11" s="5">
+        <v>29.760862714890941</v>
+      </c>
+      <c r="J11" s="5">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="20">
+        <v>2</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="5">
+        <v>25</v>
+      </c>
+      <c r="G12" s="5">
+        <v>85</v>
+      </c>
+      <c r="H12" s="5">
+        <v>169</v>
+      </c>
+      <c r="I12" s="5">
+        <v>29.760862714890941</v>
+      </c>
+      <c r="J12" s="5">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="20">
+        <v>3</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="5">
+        <v>25</v>
+      </c>
+      <c r="G13" s="5">
+        <v>85</v>
+      </c>
+      <c r="H13" s="5">
+        <v>169</v>
+      </c>
+      <c r="I13" s="5">
+        <v>29.760862714890941</v>
+      </c>
+      <c r="J13" s="5">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="19">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14">
+        <v>71</v>
+      </c>
+      <c r="G14">
+        <v>60</v>
+      </c>
+      <c r="H14">
+        <v>169</v>
+      </c>
+      <c r="I14">
+        <v>21.007667798746546</v>
+      </c>
+      <c r="J14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="20">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15">
+        <v>71</v>
+      </c>
+      <c r="G15">
+        <v>60</v>
+      </c>
+      <c r="H15">
+        <v>169</v>
+      </c>
+      <c r="I15">
+        <v>21.007667798746546</v>
+      </c>
+      <c r="J15">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="20">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16">
+        <v>71</v>
+      </c>
+      <c r="G16">
+        <v>60</v>
+      </c>
+      <c r="H16">
+        <v>169</v>
+      </c>
+      <c r="I16">
+        <v>21.007667798746546</v>
+      </c>
+      <c r="J16">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="19">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>53</v>
+      </c>
+      <c r="G17">
+        <v>68</v>
+      </c>
+      <c r="H17">
+        <v>159</v>
+      </c>
+      <c r="I17">
+        <v>26.897670187097027</v>
+      </c>
+      <c r="J17">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="20">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18">
+        <v>53</v>
+      </c>
+      <c r="G18">
+        <v>68</v>
+      </c>
+      <c r="H18">
+        <v>159</v>
+      </c>
+      <c r="I18">
+        <v>26.897670187097027</v>
+      </c>
+      <c r="J18">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="20">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19">
+        <v>53</v>
+      </c>
+      <c r="G19">
+        <v>68</v>
+      </c>
+      <c r="H19">
+        <v>159</v>
+      </c>
+      <c r="I19">
+        <v>26.897670187097027</v>
+      </c>
+      <c r="J19">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="19">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20">
+        <v>32</v>
+      </c>
+      <c r="G20">
+        <v>59.4</v>
+      </c>
+      <c r="H20">
+        <v>177.8</v>
+      </c>
+      <c r="I20">
+        <v>18.789833498034341</v>
+      </c>
+      <c r="J20">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="20">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21">
+        <v>32</v>
+      </c>
+      <c r="G21">
+        <v>59.4</v>
+      </c>
+      <c r="H21">
+        <v>177.8</v>
+      </c>
+      <c r="I21">
+        <v>18.789833498034341</v>
+      </c>
+      <c r="J21">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="20">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22">
+        <v>32</v>
+      </c>
+      <c r="G22">
+        <v>59.4</v>
+      </c>
+      <c r="H22">
+        <v>177.8</v>
+      </c>
+      <c r="I22">
+        <v>18.789833498034341</v>
+      </c>
+      <c r="J22">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="19">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23">
+        <v>47</v>
+      </c>
+      <c r="G23">
+        <v>53.9</v>
+      </c>
+      <c r="H23">
+        <v>161.30000000000001</v>
+      </c>
+      <c r="I23">
+        <v>20.716673924549021</v>
+      </c>
+      <c r="J23">
+        <v>85.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="20">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24">
+        <v>47</v>
+      </c>
+      <c r="G24">
+        <v>53.9</v>
+      </c>
+      <c r="H24">
+        <v>161.30000000000001</v>
+      </c>
+      <c r="I24">
+        <v>20.716673924549021</v>
+      </c>
+      <c r="J24">
+        <v>85.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="20">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25">
+        <v>47</v>
+      </c>
+      <c r="G25">
+        <v>53.9</v>
+      </c>
+      <c r="H25">
+        <v>161.30000000000001</v>
+      </c>
+      <c r="I25">
+        <v>20.716673924549021</v>
+      </c>
+      <c r="J25">
+        <v>85.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="19">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26">
+        <v>28</v>
+      </c>
+      <c r="G26">
+        <v>90.2</v>
+      </c>
+      <c r="H26">
+        <v>181.3</v>
+      </c>
+      <c r="I26">
+        <v>27.44169476499474</v>
+      </c>
+      <c r="J26">
+        <v>95.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="20">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27">
+        <v>28</v>
+      </c>
+      <c r="G27">
+        <v>90.2</v>
+      </c>
+      <c r="H27">
+        <v>181.3</v>
+      </c>
+      <c r="I27">
+        <v>27.44169476499474</v>
+      </c>
+      <c r="J27">
+        <v>95.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="20">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28">
+        <v>28</v>
+      </c>
+      <c r="G28">
+        <v>90.2</v>
+      </c>
+      <c r="H28">
+        <v>181.3</v>
+      </c>
+      <c r="I28">
+        <v>27.44169476499474</v>
+      </c>
+      <c r="J28">
+        <v>95.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="19">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29">
+        <v>38</v>
+      </c>
+      <c r="G29">
+        <v>55</v>
+      </c>
+      <c r="H29">
+        <v>152</v>
+      </c>
+      <c r="I29">
+        <v>23.80540166204986</v>
+      </c>
+      <c r="J29">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="20">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30">
+        <v>38</v>
+      </c>
+      <c r="G30">
+        <v>55</v>
+      </c>
+      <c r="H30">
+        <v>152</v>
+      </c>
+      <c r="I30">
+        <v>23.80540166204986</v>
+      </c>
+      <c r="J30">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="20">
+        <v>3</v>
+      </c>
+      <c r="D31" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31">
+        <v>38</v>
+      </c>
+      <c r="G31">
+        <v>55</v>
+      </c>
+      <c r="H31">
+        <v>152</v>
+      </c>
+      <c r="I31">
+        <v>23.80540166204986</v>
+      </c>
+      <c r="J31">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="19">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32">
+        <v>60</v>
+      </c>
+      <c r="G32">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="H32">
+        <v>164.1</v>
+      </c>
+      <c r="I32">
+        <v>27.814077190934174</v>
+      </c>
+      <c r="J32">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="20">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33">
+        <v>60</v>
+      </c>
+      <c r="G33">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="H33">
+        <v>164.1</v>
+      </c>
+      <c r="I33">
+        <v>27.814077190934174</v>
+      </c>
+      <c r="J33">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="20">
+        <v>3</v>
+      </c>
+      <c r="D34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34">
+        <v>60</v>
+      </c>
+      <c r="G34">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="H34">
+        <v>164.1</v>
+      </c>
+      <c r="I34">
+        <v>27.814077190934174</v>
+      </c>
+      <c r="J34">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="19">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35">
+        <v>48</v>
+      </c>
+      <c r="G35">
+        <v>69.899200000000008</v>
+      </c>
+      <c r="H35">
+        <v>158</v>
+      </c>
+      <c r="I35">
+        <v>28</v>
+      </c>
+      <c r="J35">
+        <v>95.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="20">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36">
+        <v>48</v>
+      </c>
+      <c r="G36">
+        <v>69.899200000000008</v>
+      </c>
+      <c r="H36">
+        <v>158</v>
+      </c>
+      <c r="I36">
+        <v>28</v>
+      </c>
+      <c r="J36">
+        <v>95.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="20">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37">
+        <v>48</v>
+      </c>
+      <c r="G37">
+        <v>69.899200000000008</v>
+      </c>
+      <c r="H37">
+        <v>158</v>
+      </c>
+      <c r="I37">
+        <v>28</v>
+      </c>
+      <c r="J37">
+        <v>95.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="19">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38">
+        <v>43</v>
+      </c>
+      <c r="G38">
+        <v>80</v>
+      </c>
+      <c r="H38">
+        <v>183</v>
+      </c>
+      <c r="I38">
+        <v>23.888440980620498</v>
+      </c>
+      <c r="J38">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="20">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39">
+        <v>43</v>
+      </c>
+      <c r="G39">
+        <v>80</v>
+      </c>
+      <c r="H39">
+        <v>183</v>
+      </c>
+      <c r="I39">
+        <v>23.888440980620498</v>
+      </c>
+      <c r="J39">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="20">
+        <v>3</v>
+      </c>
+      <c r="D40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40">
+        <v>43</v>
+      </c>
+      <c r="G40">
+        <v>80</v>
+      </c>
+      <c r="H40">
+        <v>183</v>
+      </c>
+      <c r="I40">
+        <v>23.888440980620498</v>
+      </c>
+      <c r="J40">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="19">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41">
+        <v>62</v>
+      </c>
+      <c r="G41">
+        <v>90.723500000000016</v>
+      </c>
+      <c r="H41">
+        <v>161</v>
+      </c>
+      <c r="I41">
+        <v>35</v>
+      </c>
+      <c r="J41">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="20">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42">
+        <v>62</v>
+      </c>
+      <c r="G42">
+        <v>90.723500000000016</v>
+      </c>
+      <c r="H42">
+        <v>161</v>
+      </c>
+      <c r="I42">
+        <v>35</v>
+      </c>
+      <c r="J42">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="20">
+        <v>3</v>
+      </c>
+      <c r="D43" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43">
+        <v>62</v>
+      </c>
+      <c r="G43">
+        <v>90.723500000000016</v>
+      </c>
+      <c r="H43">
+        <v>161</v>
+      </c>
+      <c r="I43">
+        <v>35</v>
+      </c>
+      <c r="J43">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" s="19">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44">
+        <v>22</v>
+      </c>
+      <c r="G44">
+        <v>69.634799999999998</v>
+      </c>
+      <c r="H44">
+        <v>174</v>
+      </c>
+      <c r="I44">
+        <v>23</v>
+      </c>
+      <c r="J44">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" s="20">
+        <v>2</v>
+      </c>
+      <c r="D45" t="s">
+        <v>29</v>
+      </c>
+      <c r="E45" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45">
+        <v>22</v>
+      </c>
+      <c r="G45">
+        <v>69.634799999999998</v>
+      </c>
+      <c r="H45">
+        <v>174</v>
+      </c>
+      <c r="I45">
+        <v>23</v>
+      </c>
+      <c r="J45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" s="20">
+        <v>3</v>
+      </c>
+      <c r="D46" t="s">
+        <v>29</v>
+      </c>
+      <c r="E46" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46">
+        <v>22</v>
+      </c>
+      <c r="G46">
+        <v>69.634799999999998</v>
+      </c>
+      <c r="H46">
+        <v>174</v>
+      </c>
+      <c r="I46">
+        <v>23</v>
+      </c>
+      <c r="J46">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="19">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47">
+        <v>29</v>
+      </c>
+      <c r="G47">
+        <v>82.378399999999999</v>
+      </c>
+      <c r="H47">
+        <v>178</v>
+      </c>
+      <c r="I47">
+        <v>26</v>
+      </c>
+      <c r="J47">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="20">
+        <v>2</v>
+      </c>
+      <c r="D48" t="s">
+        <v>30</v>
+      </c>
+      <c r="E48" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48">
+        <v>29</v>
+      </c>
+      <c r="G48">
+        <v>82.378399999999999</v>
+      </c>
+      <c r="H48">
+        <v>178</v>
+      </c>
+      <c r="I48">
+        <v>26</v>
+      </c>
+      <c r="J48">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" s="20">
+        <v>3</v>
+      </c>
+      <c r="D49" t="s">
+        <v>30</v>
+      </c>
+      <c r="E49" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49">
+        <v>29</v>
+      </c>
+      <c r="G49">
+        <v>82.378399999999999</v>
+      </c>
+      <c r="H49">
+        <v>178</v>
+      </c>
+      <c r="I49">
+        <v>26</v>
+      </c>
+      <c r="J49">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:J49">
+    <sortCondition ref="B2:B49"/>
+  </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDEA0401-A6D3-450D-B73D-29B36405E30A}">
   <dimension ref="A1:B17"/>
   <sheetViews>
@@ -2249,11 +4091,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBECE233-8A82-485F-BD4D-7571C7A76DC4}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>